<commit_message>
complete with challenge questions
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandoncoughlin/Desktop/NSS/DA12/projects/excel-lookups-da12-brandonwcoughlin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CF0942-45BE-BA4B-8812-032850A5D0E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165A7898-F4A5-3746-ACD5-7E88E5771239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
-    <sheet name="data_dictionary" sheetId="2" r:id="rId2"/>
+    <sheet name="duplicate table" sheetId="3" r:id="rId2"/>
+    <sheet name="data_dictionary" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -33,8 +34,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="90">
   <si>
     <t>Department</t>
   </si>
@@ -314,7 +337,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,6 +482,21 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -767,7 +805,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -810,8 +848,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -824,8 +863,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -865,11 +908,340 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -880,6 +1252,1008 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$B$82:$B$83</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Codes Administration</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Budget</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$B$84:$B$86</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>9349400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11073700</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10790500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FD96-E445-A294-A98480B83A0D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$C$82:$C$83</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Codes Administration</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$C$84:$C$86</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>8952825.2799999993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9929059.5199999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9993599.52999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FD96-E445-A294-A98480B83A0D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2068487471"/>
+        <c:axId val="1887516895"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2068487471"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1887516895"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1887516895"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2068487471"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1860550</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05C72483-E920-E2FC-68B7-911DD80D064D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82864C22-FD07-ED4F-9686-8075D17E4C91}" name="Table1" displayName="Table1" ref="A1:P52" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:P52" xr:uid="{82864C22-FD07-ED4F-9686-8075D17E4C91}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P52">
+    <sortCondition descending="1" ref="K1:K52"/>
+  </sortState>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{98EA2428-68DF-3D48-83B5-D9F7E32D7208}" name="Department" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{A82FF0B2-2558-7A4C-AE29-90627A83E27E}" name="FY17_Budget" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{FFFA34F7-EC56-DE41-9020-25BD653FCB74}" name="FY17_Actual" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{1923ED7A-E8C6-CD4C-A9BF-493C7CAAA559}" name="FY17_diff" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{6DBE58B8-8652-4149-AB6C-DE5A767F1213}" name="FY17_diff_pct" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{55EB89AB-08FE-1044-9180-D2F2BB7B2298}" name="FY17_rank" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{D0F19D3B-3574-0A4C-8D46-843E7DFE548E}" name="FY18_Budget" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{EB6C3F4A-0F68-CE48-A6DC-A338FAAD9479}" name="FY18_Actual" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{0797AEE4-9959-FB4C-9C9D-CA874121C2C0}" name="FY18_diff" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{6F64EB39-B3CD-1649-AAFD-1A6CF7FB10B2}" name="FY18_diff_pct" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{87696B01-46D1-334D-8897-EB82C74F163F}" name="FY18_rank" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{E3BE8E29-714D-3744-A5AD-778C66A640B0}" name="FY19_Budget" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{12075FB4-F4CE-F74B-ACEB-59C26295CCDC}" name="FY19_Actual" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{AEE063E7-3837-B948-AC5A-3DD3FAC37DDB}" name="FY19_diff" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{D7BD95EA-A89B-CF4A-A72B-A7025AEE2F87}" name="FY19_diff_pct" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{5D6FA727-97DC-164D-BF3F-0005FBEC4243}" name="FY19_rank" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1181,8 +2555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1263,12 +2637,12 @@
         <f>SUM(IFERROR(C2-B2,0))</f>
         <v>-15396420.870000005</v>
       </c>
-      <c r="E2" s="5">
-        <f>IFERROR(D2/B2,0)</f>
+      <c r="E2" s="5" cm="1">
+        <f t="array" ref="E2">IFERROR(D2/B2,no value)</f>
         <v>-4.3170750765267295E-2</v>
       </c>
       <c r="F2">
-        <f>RANK(E2,$E$2:$E$52,0)</f>
+        <f>_xlfn.RANK.EQ(E2,E2:E52,0)</f>
         <v>38</v>
       </c>
       <c r="G2">
@@ -1327,7 +2701,7 @@
         <v>-2.3069981751824741E-2</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F52" si="2">RANK(E3,$E$2:$E$52,0)</f>
+        <f t="shared" ref="F3:F52" si="2">_xlfn.RANK.EQ(E3,E3:E53,0)</f>
         <v>30</v>
       </c>
       <c r="G3">
@@ -1446,7 +2820,7 @@
       </c>
       <c r="F5">
         <f t="shared" si="2"/>
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G5">
         <v>7968300</v>
@@ -1505,7 +2879,7 @@
       </c>
       <c r="F6">
         <f t="shared" si="2"/>
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G6">
         <v>428500</v>
@@ -1564,7 +2938,7 @@
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G7">
         <v>3390900</v>
@@ -1623,7 +2997,7 @@
       </c>
       <c r="F8">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G8">
         <v>1590700</v>
@@ -1682,7 +3056,7 @@
       </c>
       <c r="F9">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G9">
         <v>11073700</v>
@@ -1741,7 +3115,7 @@
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G10">
         <v>495200</v>
@@ -1859,7 +3233,7 @@
       </c>
       <c r="F12">
         <f t="shared" si="2"/>
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G12">
         <v>4700400</v>
@@ -1918,7 +3292,7 @@
       </c>
       <c r="F13">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G13">
         <v>6223700</v>
@@ -1977,7 +3351,7 @@
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G14">
         <v>530500</v>
@@ -2095,7 +3469,7 @@
       </c>
       <c r="F16">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G16">
         <v>7352500</v>
@@ -2154,7 +3528,7 @@
       </c>
       <c r="F17">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G17">
         <v>15309700</v>
@@ -2213,7 +3587,7 @@
       </c>
       <c r="F18">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="G18">
         <v>2861000</v>
@@ -2272,7 +3646,7 @@
       </c>
       <c r="F19">
         <f t="shared" si="2"/>
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G19">
         <v>9713300</v>
@@ -2331,7 +3705,7 @@
       </c>
       <c r="F20">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G20">
         <v>131849400</v>
@@ -2390,7 +3764,7 @@
       </c>
       <c r="F21">
         <f t="shared" si="2"/>
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="G21">
         <v>24497400</v>
@@ -2449,7 +3823,7 @@
       </c>
       <c r="F22">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G22">
         <v>11980700</v>
@@ -2508,7 +3882,7 @@
       </c>
       <c r="F23">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="G23">
         <v>22683800</v>
@@ -2567,7 +3941,7 @@
       </c>
       <c r="F24">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G24">
         <v>1112700</v>
@@ -2626,7 +4000,7 @@
       </c>
       <c r="F25">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G25">
         <v>505200</v>
@@ -2685,7 +4059,7 @@
       </c>
       <c r="F26">
         <f t="shared" si="2"/>
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="G26">
         <v>5442200</v>
@@ -2744,7 +4118,7 @@
       </c>
       <c r="F27">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -2803,7 +4177,7 @@
       </c>
       <c r="F28">
         <f t="shared" si="2"/>
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="G28">
         <v>1545700</v>
@@ -2862,7 +4236,7 @@
       </c>
       <c r="F29">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="G29">
         <v>2779500</v>
@@ -2921,7 +4295,7 @@
       </c>
       <c r="F30">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G30">
         <v>12735900</v>
@@ -2980,7 +4354,7 @@
       </c>
       <c r="F31">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="G31">
         <v>1823300</v>
@@ -3039,7 +4413,7 @@
       </c>
       <c r="F32">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G32">
         <v>6195500</v>
@@ -3098,7 +4472,7 @@
       </c>
       <c r="F33">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G33">
         <v>979671000</v>
@@ -3157,7 +4531,7 @@
       </c>
       <c r="F34">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="G34">
         <v>4350600</v>
@@ -3216,7 +4590,7 @@
       </c>
       <c r="F35">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -3275,7 +4649,7 @@
       </c>
       <c r="F36">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="G36">
         <v>898700</v>
@@ -3334,7 +4708,7 @@
       </c>
       <c r="F37">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="G37">
         <v>2229200</v>
@@ -3393,7 +4767,7 @@
       </c>
       <c r="F38">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="G38">
         <v>792800</v>
@@ -3452,7 +4826,7 @@
       </c>
       <c r="F39">
         <f t="shared" si="2"/>
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="G39">
         <v>1294400</v>
@@ -3511,7 +4885,7 @@
       </c>
       <c r="F40">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="G40">
         <v>39964900</v>
@@ -3570,7 +4944,7 @@
       </c>
       <c r="F41">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="G41">
         <v>5089500</v>
@@ -3629,7 +5003,7 @@
       </c>
       <c r="F42">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G42">
         <v>199130300</v>
@@ -3688,7 +5062,7 @@
       </c>
       <c r="F43">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="G43">
         <v>8560800</v>
@@ -3747,7 +5121,7 @@
       </c>
       <c r="F44">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G44">
         <v>31040700</v>
@@ -3806,7 +5180,7 @@
       </c>
       <c r="F45">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G45">
         <v>56792200</v>
@@ -3865,7 +5239,7 @@
       </c>
       <c r="F46">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G46">
         <v>266000</v>
@@ -3924,7 +5298,7 @@
       </c>
       <c r="F47">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G47">
         <v>73467000</v>
@@ -3983,7 +5357,7 @@
       </c>
       <c r="F48">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="G48">
         <v>7214700</v>
@@ -4042,7 +5416,7 @@
       </c>
       <c r="F49">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="G49">
         <v>102600</v>
@@ -4101,7 +5475,7 @@
       </c>
       <c r="F50">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G50">
         <v>859100</v>
@@ -4160,7 +5534,7 @@
       </c>
       <c r="F51">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="G51">
         <v>8925500</v>
@@ -4219,7 +5593,7 @@
       </c>
       <c r="F52">
         <f t="shared" si="2"/>
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="G52">
         <v>2440700</v>
@@ -4631,7 +6005,7 @@
         <v>0</v>
       </c>
       <c r="B82" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -4648,11 +6022,11 @@
       </c>
       <c r="B84" s="6">
         <f>INDEX(B2:B52,MATCH($B$82,A2:A52))</f>
-        <v>3130600</v>
+        <v>9349400</v>
       </c>
       <c r="C84" s="6">
         <f>INDEX(C2:C52,MATCH($B$82,$A$2:$A$52))</f>
-        <v>3115157.5599999898</v>
+        <v>8952825.2799999993</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -4661,11 +6035,11 @@
       </c>
       <c r="B85" s="6">
         <f>INDEX(G2:G52,MATCH($B$82,A2:A52))</f>
-        <v>3652300</v>
+        <v>11073700</v>
       </c>
       <c r="C85" s="6">
         <f>INDEX(H2:H52,MATCH($B$82,$A$2:$A$52))</f>
-        <v>3589693.2099999902</v>
+        <v>9929059.5199999996</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
@@ -4674,11 +6048,11 @@
       </c>
       <c r="B86" s="6">
         <f>INDEX(L2:L52,MATCH(B82,A2:A52))</f>
-        <v>3662400</v>
+        <v>10790500</v>
       </c>
       <c r="C86" s="6">
         <f>INDEX(M2:M52,MATCH(B82,A2:A52))</f>
-        <v>3564983.04999999</v>
+        <v>9993599.52999999</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -4726,25 +6100,82 @@
       <c r="A91" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C91" s="5"/>
-      <c r="E91" s="5"/>
-      <c r="G91" s="5"/>
+      <c r="B91" t="str">
+        <f>_xlfn.XLOOKUP($B$89,$F$2:$F$52,$A$2:$A$52)</f>
+        <v>Debt Service</v>
+      </c>
+      <c r="C91" s="13">
+        <f>_xlfn.XLOOKUP($B$91,$A$2:$A$52,E2:E52)</f>
+        <v>3.1837408866824991E-3</v>
+      </c>
+      <c r="D91" t="str">
+        <f>_xlfn.XLOOKUP($D$89,F2:F52,$A$2:$A$52)</f>
+        <v>Community Oversight Board</v>
+      </c>
+      <c r="E91" s="5">
+        <f>_xlfn.XLOOKUP(D$91,$A$2:$A$52,E2:E52)</f>
+        <v>0</v>
+      </c>
+      <c r="F91" t="str">
+        <f>_xlfn.XLOOKUP(F$89,F$2:F$52,$A$2:$A$52)</f>
+        <v>Sheriff</v>
+      </c>
+      <c r="G91" s="5">
+        <f>_xlfn.XLOOKUP($F$91,A2:A52,E2:E52)</f>
+        <v>-1.7435939690898361E-4</v>
+      </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C92" s="5"/>
+      <c r="B92" t="str">
+        <f>_xlfn.XLOOKUP($B$89,$K$2:$K$52,$A$2:$A$52)</f>
+        <v>Community Oversight Board</v>
+      </c>
+      <c r="C92" s="13">
+        <f>_xlfn.XLOOKUP($B$92,$A$2:$A$52,J2:J52)</f>
+        <v>0</v>
+      </c>
+      <c r="D92" t="e">
+        <f>_xlfn.XLOOKUP($D$89,K2:K52,$A$2:$A$52)</f>
+        <v>#N/A</v>
+      </c>
       <c r="E92" s="5"/>
-      <c r="G92" s="5"/>
+      <c r="F92" t="e">
+        <f>_xlfn.XLOOKUP(F$89,K$2:K$52,$A$2:$A$52)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G92" s="5">
+        <f>_xlfn.XLOOKUP($F$91,A3:A53,J2:J52)</f>
+        <v>-3.2319887218048821E-2</v>
+      </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C93" s="5"/>
+      <c r="B93" t="str">
+        <f>_xlfn.XLOOKUP($B$89,$P$2:$P$52,$A$2:$A$52)</f>
+        <v>Information Technology Service</v>
+      </c>
+      <c r="C93" s="13">
+        <f>_xlfn.XLOOKUP($B$93,$A$2:$A$52,O2:O52)</f>
+        <v>0</v>
+      </c>
+      <c r="D93" t="e">
+        <f>_xlfn.XLOOKUP($D$89,P2:P52,$A$2:$A$52)</f>
+        <v>#N/A</v>
+      </c>
       <c r="E93" s="5"/>
-      <c r="G93" s="5"/>
+      <c r="F93" t="e">
+        <f>_xlfn.XLOOKUP(F$89,K$2:K$52,$A$2:$A$52)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G93" s="5">
+        <f>_xlfn.XLOOKUP($F$91,A4:A54,O4:O54)</f>
+        <v>-2.9266019117572752E-4</v>
+      </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
@@ -4822,10 +6253,2647 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020A7E86-7E17-9A4F-A0DB-3E0F5F177375}">
+  <dimension ref="A1:P52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="11.5" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" customWidth="1"/>
+    <col min="13" max="13" width="13.1640625" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14" customWidth="1"/>
+    <col min="16" max="16" width="11.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="11">
+        <v>798200</v>
+      </c>
+      <c r="C2" s="11">
+        <v>735423.28</v>
+      </c>
+      <c r="D2" s="11">
+        <v>-62776.72</v>
+      </c>
+      <c r="E2" s="12">
+        <v>-7.8600000000000003E-2</v>
+      </c>
+      <c r="F2" s="11">
+        <v>42</v>
+      </c>
+      <c r="G2" s="11">
+        <v>898700</v>
+      </c>
+      <c r="H2" s="11">
+        <v>740966.95</v>
+      </c>
+      <c r="I2" s="11">
+        <v>-157733.04999999999</v>
+      </c>
+      <c r="J2" s="12">
+        <v>-0.17549999999999999</v>
+      </c>
+      <c r="K2" s="11">
+        <v>51</v>
+      </c>
+      <c r="L2" s="11">
+        <v>878300</v>
+      </c>
+      <c r="M2" s="11">
+        <v>777215.29</v>
+      </c>
+      <c r="N2" s="11">
+        <v>-101084.71</v>
+      </c>
+      <c r="O2" s="12">
+        <v>-0.11509999999999999</v>
+      </c>
+      <c r="P2" s="11">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="11">
+        <v>1382900</v>
+      </c>
+      <c r="C3" s="11">
+        <v>1250442.02</v>
+      </c>
+      <c r="D3" s="11">
+        <v>-132457.98000000001</v>
+      </c>
+      <c r="E3" s="12">
+        <v>-9.5799999999999996E-2</v>
+      </c>
+      <c r="F3" s="11">
+        <v>49</v>
+      </c>
+      <c r="G3" s="11">
+        <v>1545700</v>
+      </c>
+      <c r="H3" s="11">
+        <v>1281335.23</v>
+      </c>
+      <c r="I3" s="11">
+        <v>-264364.77</v>
+      </c>
+      <c r="J3" s="12">
+        <v>-0.17100000000000001</v>
+      </c>
+      <c r="K3" s="11">
+        <v>50</v>
+      </c>
+      <c r="L3" s="11">
+        <v>1525900</v>
+      </c>
+      <c r="M3" s="11">
+        <v>1393285.06</v>
+      </c>
+      <c r="N3" s="11">
+        <v>-132614.94</v>
+      </c>
+      <c r="O3" s="12">
+        <v>-8.6900000000000005E-2</v>
+      </c>
+      <c r="P3" s="11">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="11">
+        <v>883900</v>
+      </c>
+      <c r="C4" s="11">
+        <v>813108.87</v>
+      </c>
+      <c r="D4" s="11">
+        <v>-70791.13</v>
+      </c>
+      <c r="E4" s="12">
+        <v>-8.0100000000000005E-2</v>
+      </c>
+      <c r="F4" s="11">
+        <v>44</v>
+      </c>
+      <c r="G4" s="11">
+        <v>1294400</v>
+      </c>
+      <c r="H4" s="11">
+        <v>1114242.28</v>
+      </c>
+      <c r="I4" s="11">
+        <v>-180157.72</v>
+      </c>
+      <c r="J4" s="12">
+        <v>-0.13919999999999999</v>
+      </c>
+      <c r="K4" s="11">
+        <v>49</v>
+      </c>
+      <c r="L4" s="11">
+        <v>1759500</v>
+      </c>
+      <c r="M4" s="11">
+        <v>1680463.87</v>
+      </c>
+      <c r="N4" s="11">
+        <v>-79036.13</v>
+      </c>
+      <c r="O4" s="12">
+        <v>-4.4900000000000002E-2</v>
+      </c>
+      <c r="P4" s="11">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="11">
+        <v>1552100</v>
+      </c>
+      <c r="C5" s="11">
+        <v>1315623.31</v>
+      </c>
+      <c r="D5" s="11">
+        <v>-236476.69</v>
+      </c>
+      <c r="E5" s="12">
+        <v>-0.15240000000000001</v>
+      </c>
+      <c r="F5" s="11">
+        <v>51</v>
+      </c>
+      <c r="G5" s="11">
+        <v>1590700</v>
+      </c>
+      <c r="H5" s="11">
+        <v>1383905.99</v>
+      </c>
+      <c r="I5" s="11">
+        <v>-206794.01</v>
+      </c>
+      <c r="J5" s="12">
+        <v>-0.13</v>
+      </c>
+      <c r="K5" s="11">
+        <v>48</v>
+      </c>
+      <c r="L5" s="11">
+        <v>1579300</v>
+      </c>
+      <c r="M5" s="11">
+        <v>1337735.32</v>
+      </c>
+      <c r="N5" s="11">
+        <v>-241564.68</v>
+      </c>
+      <c r="O5" s="12">
+        <v>-0.153</v>
+      </c>
+      <c r="P5" s="11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="11">
+        <v>7670700</v>
+      </c>
+      <c r="C6" s="11">
+        <v>6947552.6699999999</v>
+      </c>
+      <c r="D6" s="11">
+        <v>-723147.33</v>
+      </c>
+      <c r="E6" s="12">
+        <v>-9.4299999999999995E-2</v>
+      </c>
+      <c r="F6" s="11">
+        <v>48</v>
+      </c>
+      <c r="G6" s="11">
+        <v>7968300</v>
+      </c>
+      <c r="H6" s="11">
+        <v>7020609.3200000003</v>
+      </c>
+      <c r="I6" s="11">
+        <v>-947690.68</v>
+      </c>
+      <c r="J6" s="12">
+        <v>-0.11890000000000001</v>
+      </c>
+      <c r="K6" s="11">
+        <v>47</v>
+      </c>
+      <c r="L6" s="11">
+        <v>7759600</v>
+      </c>
+      <c r="M6" s="11">
+        <v>7497322.9100000001</v>
+      </c>
+      <c r="N6" s="11">
+        <v>-262277.09000000003</v>
+      </c>
+      <c r="O6" s="12">
+        <v>-3.3799999999999997E-2</v>
+      </c>
+      <c r="P6" s="11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="11">
+        <v>4280900</v>
+      </c>
+      <c r="C7" s="11">
+        <v>4066595.33</v>
+      </c>
+      <c r="D7" s="11">
+        <v>-214304.67</v>
+      </c>
+      <c r="E7" s="12">
+        <v>-5.0099999999999999E-2</v>
+      </c>
+      <c r="F7" s="11">
+        <v>39</v>
+      </c>
+      <c r="G7" s="11">
+        <v>4700400</v>
+      </c>
+      <c r="H7" s="11">
+        <v>4205555.5999999996</v>
+      </c>
+      <c r="I7" s="11">
+        <v>-494844.4</v>
+      </c>
+      <c r="J7" s="12">
+        <v>-0.1053</v>
+      </c>
+      <c r="K7" s="11">
+        <v>46</v>
+      </c>
+      <c r="L7" s="11">
+        <v>4677800</v>
+      </c>
+      <c r="M7" s="11">
+        <v>4371713.1399999997</v>
+      </c>
+      <c r="N7" s="11">
+        <v>-306086.86</v>
+      </c>
+      <c r="O7" s="12">
+        <v>-6.54E-2</v>
+      </c>
+      <c r="P7" s="11">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="11">
+        <v>9349400</v>
+      </c>
+      <c r="C8" s="11">
+        <v>8952825.2799999993</v>
+      </c>
+      <c r="D8" s="11">
+        <v>-396574.71999999997</v>
+      </c>
+      <c r="E8" s="12">
+        <v>-4.24E-2</v>
+      </c>
+      <c r="F8" s="11">
+        <v>36</v>
+      </c>
+      <c r="G8" s="11">
+        <v>11073700</v>
+      </c>
+      <c r="H8" s="11">
+        <v>9929059.5199999996</v>
+      </c>
+      <c r="I8" s="11">
+        <v>-1144640.48</v>
+      </c>
+      <c r="J8" s="12">
+        <v>-0.10340000000000001</v>
+      </c>
+      <c r="K8" s="11">
+        <v>45</v>
+      </c>
+      <c r="L8" s="11">
+        <v>10790500</v>
+      </c>
+      <c r="M8" s="11">
+        <v>9993599.5299999993</v>
+      </c>
+      <c r="N8" s="11">
+        <v>-796900.47</v>
+      </c>
+      <c r="O8" s="12">
+        <v>-7.3899999999999993E-2</v>
+      </c>
+      <c r="P8" s="11">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="11">
+        <v>3329000</v>
+      </c>
+      <c r="C9" s="11">
+        <v>2946071.21</v>
+      </c>
+      <c r="D9" s="11">
+        <v>-382928.79</v>
+      </c>
+      <c r="E9" s="12">
+        <v>-0.115</v>
+      </c>
+      <c r="F9" s="11">
+        <v>50</v>
+      </c>
+      <c r="G9" s="11">
+        <v>3390900</v>
+      </c>
+      <c r="H9" s="11">
+        <v>3051483.41</v>
+      </c>
+      <c r="I9" s="11">
+        <v>-339416.59</v>
+      </c>
+      <c r="J9" s="12">
+        <v>-0.10009999999999999</v>
+      </c>
+      <c r="K9" s="11">
+        <v>44</v>
+      </c>
+      <c r="L9" s="11">
+        <v>3345200</v>
+      </c>
+      <c r="M9" s="11">
+        <v>2946440.08</v>
+      </c>
+      <c r="N9" s="11">
+        <v>-398759.92</v>
+      </c>
+      <c r="O9" s="12">
+        <v>-0.1192</v>
+      </c>
+      <c r="P9" s="11">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="11">
+        <v>2451000</v>
+      </c>
+      <c r="C10" s="11">
+        <v>2254684.7999999998</v>
+      </c>
+      <c r="D10" s="11">
+        <v>-196315.2</v>
+      </c>
+      <c r="E10" s="12">
+        <v>-8.0100000000000005E-2</v>
+      </c>
+      <c r="F10" s="11">
+        <v>45</v>
+      </c>
+      <c r="G10" s="11">
+        <v>2440700</v>
+      </c>
+      <c r="H10" s="11">
+        <v>2204672.88</v>
+      </c>
+      <c r="I10" s="11">
+        <v>-236027.12</v>
+      </c>
+      <c r="J10" s="12">
+        <v>-9.6699999999999994E-2</v>
+      </c>
+      <c r="K10" s="11">
+        <v>43</v>
+      </c>
+      <c r="L10" s="11">
+        <v>2321600</v>
+      </c>
+      <c r="M10" s="11">
+        <v>2056835.26</v>
+      </c>
+      <c r="N10" s="11">
+        <v>-264764.74</v>
+      </c>
+      <c r="O10" s="12">
+        <v>-0.114</v>
+      </c>
+      <c r="P10" s="11">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="11">
+        <v>356640100</v>
+      </c>
+      <c r="C11" s="11">
+        <v>341243679.10000002</v>
+      </c>
+      <c r="D11" s="11">
+        <v>-15396420.869999999</v>
+      </c>
+      <c r="E11" s="12">
+        <v>-4.3200000000000002E-2</v>
+      </c>
+      <c r="F11" s="11">
+        <v>38</v>
+      </c>
+      <c r="G11" s="11">
+        <v>382685200</v>
+      </c>
+      <c r="H11" s="11">
+        <v>346340810.80000001</v>
+      </c>
+      <c r="I11" s="11">
+        <v>-36344389.18</v>
+      </c>
+      <c r="J11" s="12">
+        <v>-9.5000000000000001E-2</v>
+      </c>
+      <c r="K11" s="11">
+        <v>42</v>
+      </c>
+      <c r="L11" s="11">
+        <v>376548600</v>
+      </c>
+      <c r="M11" s="11">
+        <v>355279492.19999999</v>
+      </c>
+      <c r="N11" s="11">
+        <v>-21269107.77</v>
+      </c>
+      <c r="O11" s="12">
+        <v>-5.6500000000000002E-2</v>
+      </c>
+      <c r="P11" s="11">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="11">
+        <v>24332100</v>
+      </c>
+      <c r="C12" s="11">
+        <v>22408587.550000001</v>
+      </c>
+      <c r="D12" s="11">
+        <v>-1923512.45</v>
+      </c>
+      <c r="E12" s="12">
+        <v>-7.9100000000000004E-2</v>
+      </c>
+      <c r="F12" s="11">
+        <v>43</v>
+      </c>
+      <c r="G12" s="11">
+        <v>24497400</v>
+      </c>
+      <c r="H12" s="11">
+        <v>22655993.629999999</v>
+      </c>
+      <c r="I12" s="11">
+        <v>-1841406.37</v>
+      </c>
+      <c r="J12" s="12">
+        <v>-7.5200000000000003E-2</v>
+      </c>
+      <c r="K12" s="11">
+        <v>41</v>
+      </c>
+      <c r="L12" s="11">
+        <v>24323000</v>
+      </c>
+      <c r="M12" s="11">
+        <v>23434073.09</v>
+      </c>
+      <c r="N12" s="11">
+        <v>-888926.91</v>
+      </c>
+      <c r="O12" s="12">
+        <v>-3.6499999999999998E-2</v>
+      </c>
+      <c r="P12" s="11">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="11">
+        <v>8837300</v>
+      </c>
+      <c r="C13" s="11">
+        <v>8460963.1999999993</v>
+      </c>
+      <c r="D13" s="11">
+        <v>-376336.8</v>
+      </c>
+      <c r="E13" s="12">
+        <v>-4.2599999999999999E-2</v>
+      </c>
+      <c r="F13" s="11">
+        <v>37</v>
+      </c>
+      <c r="G13" s="11">
+        <v>9713300</v>
+      </c>
+      <c r="H13" s="11">
+        <v>8991707.2400000002</v>
+      </c>
+      <c r="I13" s="11">
+        <v>-721592.76</v>
+      </c>
+      <c r="J13" s="12">
+        <v>-7.4300000000000005E-2</v>
+      </c>
+      <c r="K13" s="11">
+        <v>40</v>
+      </c>
+      <c r="L13" s="11">
+        <v>9343000</v>
+      </c>
+      <c r="M13" s="11">
+        <v>8766655.9100000001</v>
+      </c>
+      <c r="N13" s="11">
+        <v>-576344.09</v>
+      </c>
+      <c r="O13" s="12">
+        <v>-6.1699999999999998E-2</v>
+      </c>
+      <c r="P13" s="11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="11">
+        <v>92200</v>
+      </c>
+      <c r="C14" s="11">
+        <v>90499.43</v>
+      </c>
+      <c r="D14" s="11">
+        <v>-1700.57</v>
+      </c>
+      <c r="E14" s="12">
+        <v>-1.84E-2</v>
+      </c>
+      <c r="F14" s="11">
+        <v>25</v>
+      </c>
+      <c r="G14" s="11">
+        <v>102600</v>
+      </c>
+      <c r="H14" s="11">
+        <v>95466.880000000005</v>
+      </c>
+      <c r="I14" s="11">
+        <v>-7133.12</v>
+      </c>
+      <c r="J14" s="12">
+        <v>-6.9500000000000006E-2</v>
+      </c>
+      <c r="K14" s="11">
+        <v>39</v>
+      </c>
+      <c r="L14" s="11">
+        <v>0</v>
+      </c>
+      <c r="M14" s="11">
+        <v>0</v>
+      </c>
+      <c r="N14" s="11">
+        <v>0</v>
+      </c>
+      <c r="O14" s="12">
+        <v>0</v>
+      </c>
+      <c r="P14" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="11">
+        <v>328800</v>
+      </c>
+      <c r="C15" s="11">
+        <v>321214.59000000003</v>
+      </c>
+      <c r="D15" s="11">
+        <v>-7585.41</v>
+      </c>
+      <c r="E15" s="12">
+        <v>-2.3099999999999999E-2</v>
+      </c>
+      <c r="F15" s="11">
+        <v>30</v>
+      </c>
+      <c r="G15" s="11">
+        <v>334800</v>
+      </c>
+      <c r="H15" s="11">
+        <v>312433.71000000002</v>
+      </c>
+      <c r="I15" s="11">
+        <v>-22366.29</v>
+      </c>
+      <c r="J15" s="12">
+        <v>-6.6799999999999998E-2</v>
+      </c>
+      <c r="K15" s="11">
+        <v>38</v>
+      </c>
+      <c r="L15" s="11">
+        <v>322700</v>
+      </c>
+      <c r="M15" s="11">
+        <v>322263.03999999998</v>
+      </c>
+      <c r="N15" s="11">
+        <v>-436.96</v>
+      </c>
+      <c r="O15" s="12">
+        <v>-1.4E-3</v>
+      </c>
+      <c r="P15" s="11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="11">
+        <v>2764700</v>
+      </c>
+      <c r="C16" s="11">
+        <v>2615303.9</v>
+      </c>
+      <c r="D16" s="11">
+        <v>-149396.1</v>
+      </c>
+      <c r="E16" s="12">
+        <v>-5.3999999999999999E-2</v>
+      </c>
+      <c r="F16" s="11">
+        <v>40</v>
+      </c>
+      <c r="G16" s="11">
+        <v>2861000</v>
+      </c>
+      <c r="H16" s="11">
+        <v>2671745.94</v>
+      </c>
+      <c r="I16" s="11">
+        <v>-189254.06</v>
+      </c>
+      <c r="J16" s="12">
+        <v>-6.6100000000000006E-2</v>
+      </c>
+      <c r="K16" s="11">
+        <v>37</v>
+      </c>
+      <c r="L16" s="11">
+        <v>2910600</v>
+      </c>
+      <c r="M16" s="11">
+        <v>2535637.09</v>
+      </c>
+      <c r="N16" s="11">
+        <v>-374962.91</v>
+      </c>
+      <c r="O16" s="12">
+        <v>-0.1288</v>
+      </c>
+      <c r="P16" s="11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="11">
+        <v>5249800</v>
+      </c>
+      <c r="C17" s="11">
+        <v>4801960.08</v>
+      </c>
+      <c r="D17" s="11">
+        <v>-447839.92</v>
+      </c>
+      <c r="E17" s="12">
+        <v>-8.5300000000000001E-2</v>
+      </c>
+      <c r="F17" s="11">
+        <v>47</v>
+      </c>
+      <c r="G17" s="11">
+        <v>5442200</v>
+      </c>
+      <c r="H17" s="11">
+        <v>5122329.03</v>
+      </c>
+      <c r="I17" s="11">
+        <v>-319870.96999999997</v>
+      </c>
+      <c r="J17" s="12">
+        <v>-5.8799999999999998E-2</v>
+      </c>
+      <c r="K17" s="11">
+        <v>36</v>
+      </c>
+      <c r="L17" s="11">
+        <v>5430700</v>
+      </c>
+      <c r="M17" s="11">
+        <v>5117235.21</v>
+      </c>
+      <c r="N17" s="11">
+        <v>-313464.78999999998</v>
+      </c>
+      <c r="O17" s="12">
+        <v>-5.7700000000000001E-2</v>
+      </c>
+      <c r="P17" s="11">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="11">
+        <v>443300</v>
+      </c>
+      <c r="C18" s="11">
+        <v>407090.37</v>
+      </c>
+      <c r="D18" s="11">
+        <v>-36209.629999999997</v>
+      </c>
+      <c r="E18" s="12">
+        <v>-8.1699999999999995E-2</v>
+      </c>
+      <c r="F18" s="11">
+        <v>46</v>
+      </c>
+      <c r="G18" s="11">
+        <v>495200</v>
+      </c>
+      <c r="H18" s="11">
+        <v>467907.84000000003</v>
+      </c>
+      <c r="I18" s="11">
+        <v>-27292.16</v>
+      </c>
+      <c r="J18" s="12">
+        <v>-5.5100000000000003E-2</v>
+      </c>
+      <c r="K18" s="11">
+        <v>35</v>
+      </c>
+      <c r="L18" s="11">
+        <v>487500</v>
+      </c>
+      <c r="M18" s="11">
+        <v>478318.92</v>
+      </c>
+      <c r="N18" s="11">
+        <v>-9181.08</v>
+      </c>
+      <c r="O18" s="12">
+        <v>-1.8800000000000001E-2</v>
+      </c>
+      <c r="P18" s="11">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="11">
+        <v>5847800</v>
+      </c>
+      <c r="C19" s="11">
+        <v>5772288.3300000001</v>
+      </c>
+      <c r="D19" s="11">
+        <v>-75511.67</v>
+      </c>
+      <c r="E19" s="12">
+        <v>-1.29E-2</v>
+      </c>
+      <c r="F19" s="11">
+        <v>19</v>
+      </c>
+      <c r="G19" s="11">
+        <v>6223700</v>
+      </c>
+      <c r="H19" s="11">
+        <v>5909077.9400000004</v>
+      </c>
+      <c r="I19" s="11">
+        <v>-314622.06</v>
+      </c>
+      <c r="J19" s="12">
+        <v>-5.0599999999999999E-2</v>
+      </c>
+      <c r="K19" s="11">
+        <v>34</v>
+      </c>
+      <c r="L19" s="11">
+        <v>6207300</v>
+      </c>
+      <c r="M19" s="11">
+        <v>6056976.6699999999</v>
+      </c>
+      <c r="N19" s="11">
+        <v>-150323.32999999999</v>
+      </c>
+      <c r="O19" s="12">
+        <v>-2.4199999999999999E-2</v>
+      </c>
+      <c r="P19" s="11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="11">
+        <v>855300</v>
+      </c>
+      <c r="C20" s="11">
+        <v>838669.82</v>
+      </c>
+      <c r="D20" s="11">
+        <v>-16630.18</v>
+      </c>
+      <c r="E20" s="12">
+        <v>-1.9400000000000001E-2</v>
+      </c>
+      <c r="F20" s="11">
+        <v>27</v>
+      </c>
+      <c r="G20" s="11">
+        <v>792800</v>
+      </c>
+      <c r="H20" s="11">
+        <v>753451.96</v>
+      </c>
+      <c r="I20" s="11">
+        <v>-39348.04</v>
+      </c>
+      <c r="J20" s="12">
+        <v>-4.9599999999999998E-2</v>
+      </c>
+      <c r="K20" s="11">
+        <v>33</v>
+      </c>
+      <c r="L20" s="11">
+        <v>777800</v>
+      </c>
+      <c r="M20" s="11">
+        <v>777663.26</v>
+      </c>
+      <c r="N20" s="11">
+        <v>-136.74</v>
+      </c>
+      <c r="O20" s="12">
+        <v>-2.0000000000000001E-4</v>
+      </c>
+      <c r="P20" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="11">
+        <v>2087800</v>
+      </c>
+      <c r="C21" s="11">
+        <v>2005447.74</v>
+      </c>
+      <c r="D21" s="11">
+        <v>-82352.259999999995</v>
+      </c>
+      <c r="E21" s="12">
+        <v>-3.9399999999999998E-2</v>
+      </c>
+      <c r="F21" s="11">
+        <v>33</v>
+      </c>
+      <c r="G21" s="11">
+        <v>2229200</v>
+      </c>
+      <c r="H21" s="11">
+        <v>2118943.21</v>
+      </c>
+      <c r="I21" s="11">
+        <v>-110256.79</v>
+      </c>
+      <c r="J21" s="12">
+        <v>-4.9500000000000002E-2</v>
+      </c>
+      <c r="K21" s="11">
+        <v>32</v>
+      </c>
+      <c r="L21" s="11">
+        <v>2296900</v>
+      </c>
+      <c r="M21" s="11">
+        <v>2108718.34</v>
+      </c>
+      <c r="N21" s="11">
+        <v>-188181.66</v>
+      </c>
+      <c r="O21" s="12">
+        <v>-8.1900000000000001E-2</v>
+      </c>
+      <c r="P21" s="11">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="11">
+        <v>4189300</v>
+      </c>
+      <c r="C22" s="11">
+        <v>4109958.22</v>
+      </c>
+      <c r="D22" s="11">
+        <v>-79341.78</v>
+      </c>
+      <c r="E22" s="12">
+        <v>-1.89E-2</v>
+      </c>
+      <c r="F22" s="11">
+        <v>26</v>
+      </c>
+      <c r="G22" s="11">
+        <v>4350600</v>
+      </c>
+      <c r="H22" s="11">
+        <v>4137588.77</v>
+      </c>
+      <c r="I22" s="11">
+        <v>-213011.23</v>
+      </c>
+      <c r="J22" s="12">
+        <v>-4.9000000000000002E-2</v>
+      </c>
+      <c r="K22" s="11">
+        <v>31</v>
+      </c>
+      <c r="L22" s="11">
+        <v>4345600</v>
+      </c>
+      <c r="M22" s="11">
+        <v>4229801.51</v>
+      </c>
+      <c r="N22" s="11">
+        <v>-115798.49</v>
+      </c>
+      <c r="O22" s="12">
+        <v>-2.6599999999999999E-2</v>
+      </c>
+      <c r="P22" s="11">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="11">
+        <v>38381900</v>
+      </c>
+      <c r="C23" s="11">
+        <v>37565141.859999999</v>
+      </c>
+      <c r="D23" s="11">
+        <v>-816758.14</v>
+      </c>
+      <c r="E23" s="12">
+        <v>-2.1299999999999999E-2</v>
+      </c>
+      <c r="F23" s="11">
+        <v>29</v>
+      </c>
+      <c r="G23" s="11">
+        <v>39964900</v>
+      </c>
+      <c r="H23" s="11">
+        <v>38095240.189999998</v>
+      </c>
+      <c r="I23" s="11">
+        <v>-1869659.81</v>
+      </c>
+      <c r="J23" s="12">
+        <v>-4.6800000000000001E-2</v>
+      </c>
+      <c r="K23" s="11">
+        <v>30</v>
+      </c>
+      <c r="L23" s="11">
+        <v>40216700</v>
+      </c>
+      <c r="M23" s="11">
+        <v>39606263.710000001</v>
+      </c>
+      <c r="N23" s="11">
+        <v>-610436.29</v>
+      </c>
+      <c r="O23" s="12">
+        <v>-1.52E-2</v>
+      </c>
+      <c r="P23" s="11">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="11">
+        <v>8135400</v>
+      </c>
+      <c r="C24" s="11">
+        <v>7968645.8300000001</v>
+      </c>
+      <c r="D24" s="11">
+        <v>-166754.17000000001</v>
+      </c>
+      <c r="E24" s="12">
+        <v>-2.0500000000000001E-2</v>
+      </c>
+      <c r="F24" s="11">
+        <v>28</v>
+      </c>
+      <c r="G24" s="11">
+        <v>8560800</v>
+      </c>
+      <c r="H24" s="11">
+        <v>8171472.0199999996</v>
+      </c>
+      <c r="I24" s="11">
+        <v>-389327.98</v>
+      </c>
+      <c r="J24" s="12">
+        <v>-4.5499999999999999E-2</v>
+      </c>
+      <c r="K24" s="11">
+        <v>29</v>
+      </c>
+      <c r="L24" s="11">
+        <v>8497500</v>
+      </c>
+      <c r="M24" s="11">
+        <v>8150982.5700000003</v>
+      </c>
+      <c r="N24" s="11">
+        <v>-346517.43</v>
+      </c>
+      <c r="O24" s="12">
+        <v>-4.0800000000000003E-2</v>
+      </c>
+      <c r="P24" s="11">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="11">
+        <v>156049100</v>
+      </c>
+      <c r="C25" s="11">
+        <v>156545919.90000001</v>
+      </c>
+      <c r="D25" s="11">
+        <v>496819.9</v>
+      </c>
+      <c r="E25" s="12">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="F25" s="11">
+        <v>1</v>
+      </c>
+      <c r="G25" s="11">
+        <v>184167800</v>
+      </c>
+      <c r="H25" s="11">
+        <v>175966389.19999999</v>
+      </c>
+      <c r="I25" s="11">
+        <v>-8201410.75</v>
+      </c>
+      <c r="J25" s="12">
+        <v>-4.4499999999999998E-2</v>
+      </c>
+      <c r="K25" s="11">
+        <v>28</v>
+      </c>
+      <c r="L25" s="11">
+        <v>188953500</v>
+      </c>
+      <c r="M25" s="11">
+        <v>184450910.80000001</v>
+      </c>
+      <c r="N25" s="11">
+        <v>-4502589.1500000004</v>
+      </c>
+      <c r="O25" s="12">
+        <v>-2.3800000000000002E-2</v>
+      </c>
+      <c r="P25" s="11">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="11">
+        <v>14860800</v>
+      </c>
+      <c r="C26" s="11">
+        <v>14439480.050000001</v>
+      </c>
+      <c r="D26" s="11">
+        <v>-421319.95</v>
+      </c>
+      <c r="E26" s="12">
+        <v>-2.8400000000000002E-2</v>
+      </c>
+      <c r="F26" s="11">
+        <v>31</v>
+      </c>
+      <c r="G26" s="11">
+        <v>15309700</v>
+      </c>
+      <c r="H26" s="11">
+        <v>14645233.51</v>
+      </c>
+      <c r="I26" s="11">
+        <v>-664466.49</v>
+      </c>
+      <c r="J26" s="12">
+        <v>-4.3400000000000001E-2</v>
+      </c>
+      <c r="K26" s="11">
+        <v>27</v>
+      </c>
+      <c r="L26" s="11">
+        <v>15311800</v>
+      </c>
+      <c r="M26" s="11">
+        <v>14346057.039999999</v>
+      </c>
+      <c r="N26" s="11">
+        <v>-965742.96</v>
+      </c>
+      <c r="O26" s="12">
+        <v>-6.3100000000000003E-2</v>
+      </c>
+      <c r="P26" s="11">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="11">
+        <v>20862700</v>
+      </c>
+      <c r="C27" s="11">
+        <v>20036743.41</v>
+      </c>
+      <c r="D27" s="11">
+        <v>-825956.59</v>
+      </c>
+      <c r="E27" s="12">
+        <v>-3.9600000000000003E-2</v>
+      </c>
+      <c r="F27" s="11">
+        <v>34</v>
+      </c>
+      <c r="G27" s="11">
+        <v>22683800</v>
+      </c>
+      <c r="H27" s="11">
+        <v>21722126.219999999</v>
+      </c>
+      <c r="I27" s="11">
+        <v>-961673.78</v>
+      </c>
+      <c r="J27" s="12">
+        <v>-4.24E-2</v>
+      </c>
+      <c r="K27" s="11">
+        <v>26</v>
+      </c>
+      <c r="L27" s="11">
+        <v>23220300</v>
+      </c>
+      <c r="M27" s="11">
+        <v>22619057.440000001</v>
+      </c>
+      <c r="N27" s="11">
+        <v>-601242.56000000006</v>
+      </c>
+      <c r="O27" s="12">
+        <v>-2.5899999999999999E-2</v>
+      </c>
+      <c r="P27" s="11">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="11">
+        <v>2561800</v>
+      </c>
+      <c r="C28" s="11">
+        <v>2523884.71</v>
+      </c>
+      <c r="D28" s="11">
+        <v>-37915.29</v>
+      </c>
+      <c r="E28" s="12">
+        <v>-1.4800000000000001E-2</v>
+      </c>
+      <c r="F28" s="11">
+        <v>24</v>
+      </c>
+      <c r="G28" s="11">
+        <v>2779500</v>
+      </c>
+      <c r="H28" s="11">
+        <v>2665264.44</v>
+      </c>
+      <c r="I28" s="11">
+        <v>-114235.56</v>
+      </c>
+      <c r="J28" s="12">
+        <v>-4.1099999999999998E-2</v>
+      </c>
+      <c r="K28" s="11">
+        <v>25</v>
+      </c>
+      <c r="L28" s="11">
+        <v>2889900</v>
+      </c>
+      <c r="M28" s="11">
+        <v>2889864.67</v>
+      </c>
+      <c r="N28" s="11">
+        <v>-35.33</v>
+      </c>
+      <c r="O28" s="12">
+        <v>0</v>
+      </c>
+      <c r="P28" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="11">
+        <v>917200</v>
+      </c>
+      <c r="C29" s="11">
+        <v>904969.19</v>
+      </c>
+      <c r="D29" s="11">
+        <v>-12230.81</v>
+      </c>
+      <c r="E29" s="12">
+        <v>-1.3299999999999999E-2</v>
+      </c>
+      <c r="F29" s="11">
+        <v>21</v>
+      </c>
+      <c r="G29" s="11">
+        <v>1112700</v>
+      </c>
+      <c r="H29" s="11">
+        <v>1067214.42</v>
+      </c>
+      <c r="I29" s="11">
+        <v>-45485.58</v>
+      </c>
+      <c r="J29" s="12">
+        <v>-4.0899999999999999E-2</v>
+      </c>
+      <c r="K29" s="11">
+        <v>24</v>
+      </c>
+      <c r="L29" s="11">
+        <v>1112600</v>
+      </c>
+      <c r="M29" s="11">
+        <v>1112527.1200000001</v>
+      </c>
+      <c r="N29" s="11">
+        <v>-72.88</v>
+      </c>
+      <c r="O29" s="12">
+        <v>-1E-4</v>
+      </c>
+      <c r="P29" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="11">
+        <v>6737100</v>
+      </c>
+      <c r="C30" s="11">
+        <v>6527352.5700000003</v>
+      </c>
+      <c r="D30" s="11">
+        <v>-209747.43</v>
+      </c>
+      <c r="E30" s="12">
+        <v>-3.1099999999999999E-2</v>
+      </c>
+      <c r="F30" s="11">
+        <v>32</v>
+      </c>
+      <c r="G30" s="11">
+        <v>7214700</v>
+      </c>
+      <c r="H30" s="11">
+        <v>6922072.5599999996</v>
+      </c>
+      <c r="I30" s="11">
+        <v>-292627.44</v>
+      </c>
+      <c r="J30" s="12">
+        <v>-4.0599999999999997E-2</v>
+      </c>
+      <c r="K30" s="11">
+        <v>23</v>
+      </c>
+      <c r="L30" s="11">
+        <v>7289800</v>
+      </c>
+      <c r="M30" s="11">
+        <v>6882350.2400000002</v>
+      </c>
+      <c r="N30" s="11">
+        <v>-407449.76</v>
+      </c>
+      <c r="O30" s="12">
+        <v>-5.5899999999999998E-2</v>
+      </c>
+      <c r="P30" s="11">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="11">
+        <v>55301600</v>
+      </c>
+      <c r="C31" s="11">
+        <v>54589584.049999997</v>
+      </c>
+      <c r="D31" s="11">
+        <v>-712015.95</v>
+      </c>
+      <c r="E31" s="12">
+        <v>-1.29E-2</v>
+      </c>
+      <c r="F31" s="11">
+        <v>18</v>
+      </c>
+      <c r="G31" s="11">
+        <v>56792200</v>
+      </c>
+      <c r="H31" s="11">
+        <v>54594953.960000001</v>
+      </c>
+      <c r="I31" s="11">
+        <v>-2197246.04</v>
+      </c>
+      <c r="J31" s="12">
+        <v>-3.8699999999999998E-2</v>
+      </c>
+      <c r="K31" s="11">
+        <v>22</v>
+      </c>
+      <c r="L31" s="11">
+        <v>56027100</v>
+      </c>
+      <c r="M31" s="11">
+        <v>55386549.659999996</v>
+      </c>
+      <c r="N31" s="11">
+        <v>-640550.34</v>
+      </c>
+      <c r="O31" s="12">
+        <v>-1.14E-2</v>
+      </c>
+      <c r="P31" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="11">
+        <v>8609500</v>
+      </c>
+      <c r="C32" s="11">
+        <v>8499425.3399999999</v>
+      </c>
+      <c r="D32" s="11">
+        <v>-110074.66</v>
+      </c>
+      <c r="E32" s="12">
+        <v>-1.2800000000000001E-2</v>
+      </c>
+      <c r="F32" s="11">
+        <v>17</v>
+      </c>
+      <c r="G32" s="11">
+        <v>8925500</v>
+      </c>
+      <c r="H32" s="11">
+        <v>8599059.6199999992</v>
+      </c>
+      <c r="I32" s="11">
+        <v>-326440.38</v>
+      </c>
+      <c r="J32" s="12">
+        <v>-3.6600000000000001E-2</v>
+      </c>
+      <c r="K32" s="11">
+        <v>21</v>
+      </c>
+      <c r="L32" s="11">
+        <v>8833900</v>
+      </c>
+      <c r="M32" s="11">
+        <v>8735843.3100000005</v>
+      </c>
+      <c r="N32" s="11">
+        <v>-98056.69</v>
+      </c>
+      <c r="O32" s="12">
+        <v>-1.11E-2</v>
+      </c>
+      <c r="P32" s="11">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="11">
+        <v>1765600</v>
+      </c>
+      <c r="C33" s="11">
+        <v>1740827.69</v>
+      </c>
+      <c r="D33" s="11">
+        <v>-24772.31</v>
+      </c>
+      <c r="E33" s="12">
+        <v>-1.4E-2</v>
+      </c>
+      <c r="F33" s="11">
+        <v>23</v>
+      </c>
+      <c r="G33" s="11">
+        <v>1823300</v>
+      </c>
+      <c r="H33" s="11">
+        <v>1762676.85</v>
+      </c>
+      <c r="I33" s="11">
+        <v>-60623.15</v>
+      </c>
+      <c r="J33" s="12">
+        <v>-3.32E-2</v>
+      </c>
+      <c r="K33" s="11">
+        <v>20</v>
+      </c>
+      <c r="L33" s="11">
+        <v>1870700</v>
+      </c>
+      <c r="M33" s="11">
+        <v>1801391.34</v>
+      </c>
+      <c r="N33" s="11">
+        <v>-69308.66</v>
+      </c>
+      <c r="O33" s="12">
+        <v>-3.6999999999999998E-2</v>
+      </c>
+      <c r="P33" s="11">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A34" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="11">
+        <v>259100</v>
+      </c>
+      <c r="C34" s="11">
+        <v>258322.43</v>
+      </c>
+      <c r="D34" s="11">
+        <v>-777.57</v>
+      </c>
+      <c r="E34" s="12">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="F34" s="11">
+        <v>9</v>
+      </c>
+      <c r="G34" s="11">
+        <v>266000</v>
+      </c>
+      <c r="H34" s="11">
+        <v>257402.91</v>
+      </c>
+      <c r="I34" s="11">
+        <v>-8597.09</v>
+      </c>
+      <c r="J34" s="12">
+        <v>-3.2300000000000002E-2</v>
+      </c>
+      <c r="K34" s="11">
+        <v>19</v>
+      </c>
+      <c r="L34" s="11">
+        <v>267100</v>
+      </c>
+      <c r="M34" s="11">
+        <v>254753.16</v>
+      </c>
+      <c r="N34" s="11">
+        <v>-12346.84</v>
+      </c>
+      <c r="O34" s="12">
+        <v>-4.6199999999999998E-2</v>
+      </c>
+      <c r="P34" s="11">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="11">
+        <v>4593300</v>
+      </c>
+      <c r="C35" s="11">
+        <v>4409060.21</v>
+      </c>
+      <c r="D35" s="11">
+        <v>-184239.79</v>
+      </c>
+      <c r="E35" s="12">
+        <v>-4.0099999999999997E-2</v>
+      </c>
+      <c r="F35" s="11">
+        <v>35</v>
+      </c>
+      <c r="G35" s="11">
+        <v>5089500</v>
+      </c>
+      <c r="H35" s="11">
+        <v>4956043.67</v>
+      </c>
+      <c r="I35" s="11">
+        <v>-133456.32999999999</v>
+      </c>
+      <c r="J35" s="12">
+        <v>-2.6200000000000001E-2</v>
+      </c>
+      <c r="K35" s="11">
+        <v>18</v>
+      </c>
+      <c r="L35" s="11">
+        <v>4799900</v>
+      </c>
+      <c r="M35" s="11">
+        <v>4717822.6500000004</v>
+      </c>
+      <c r="N35" s="11">
+        <v>-82077.350000000006</v>
+      </c>
+      <c r="O35" s="12">
+        <v>-1.7100000000000001E-2</v>
+      </c>
+      <c r="P35" s="11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A36" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="11">
+        <v>5999400</v>
+      </c>
+      <c r="C36" s="11">
+        <v>5925637.7199999997</v>
+      </c>
+      <c r="D36" s="11">
+        <v>-73762.28</v>
+      </c>
+      <c r="E36" s="12">
+        <v>-1.23E-2</v>
+      </c>
+      <c r="F36" s="11">
+        <v>16</v>
+      </c>
+      <c r="G36" s="11">
+        <v>6195500</v>
+      </c>
+      <c r="H36" s="11">
+        <v>6084985.4699999997</v>
+      </c>
+      <c r="I36" s="11">
+        <v>-110514.53</v>
+      </c>
+      <c r="J36" s="12">
+        <v>-1.78E-2</v>
+      </c>
+      <c r="K36" s="11">
+        <v>17</v>
+      </c>
+      <c r="L36" s="11">
+        <v>6157400</v>
+      </c>
+      <c r="M36" s="11">
+        <v>5987572.0199999996</v>
+      </c>
+      <c r="N36" s="11">
+        <v>-169827.98</v>
+      </c>
+      <c r="O36" s="12">
+        <v>-2.76E-2</v>
+      </c>
+      <c r="P36" s="11">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="11">
+        <v>3130600</v>
+      </c>
+      <c r="C37" s="11">
+        <v>3115157.56</v>
+      </c>
+      <c r="D37" s="11">
+        <v>-15442.44</v>
+      </c>
+      <c r="E37" s="12">
+        <v>-4.8999999999999998E-3</v>
+      </c>
+      <c r="F37" s="11">
+        <v>10</v>
+      </c>
+      <c r="G37" s="11">
+        <v>3652300</v>
+      </c>
+      <c r="H37" s="11">
+        <v>3589693.21</v>
+      </c>
+      <c r="I37" s="11">
+        <v>-62606.79</v>
+      </c>
+      <c r="J37" s="12">
+        <v>-1.7100000000000001E-2</v>
+      </c>
+      <c r="K37" s="11">
+        <v>16</v>
+      </c>
+      <c r="L37" s="11">
+        <v>3662400</v>
+      </c>
+      <c r="M37" s="11">
+        <v>3564983.05</v>
+      </c>
+      <c r="N37" s="11">
+        <v>-97416.95</v>
+      </c>
+      <c r="O37" s="12">
+        <v>-2.6599999999999999E-2</v>
+      </c>
+      <c r="P37" s="11">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A38" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="11">
+        <v>484100</v>
+      </c>
+      <c r="C38" s="11">
+        <v>479149.53</v>
+      </c>
+      <c r="D38" s="11">
+        <v>-4950.47</v>
+      </c>
+      <c r="E38" s="12">
+        <v>-1.0200000000000001E-2</v>
+      </c>
+      <c r="F38" s="11">
+        <v>14</v>
+      </c>
+      <c r="G38" s="11">
+        <v>505200</v>
+      </c>
+      <c r="H38" s="11">
+        <v>497194.21</v>
+      </c>
+      <c r="I38" s="11">
+        <v>-8005.79</v>
+      </c>
+      <c r="J38" s="12">
+        <v>-1.5800000000000002E-2</v>
+      </c>
+      <c r="K38" s="11">
+        <v>15</v>
+      </c>
+      <c r="L38" s="11">
+        <v>496500</v>
+      </c>
+      <c r="M38" s="11">
+        <v>494775.1</v>
+      </c>
+      <c r="N38" s="11">
+        <v>-1724.9</v>
+      </c>
+      <c r="O38" s="12">
+        <v>-3.5000000000000001E-3</v>
+      </c>
+      <c r="P38" s="11">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A39" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="11">
+        <v>11566000</v>
+      </c>
+      <c r="C39" s="11">
+        <v>11412339.880000001</v>
+      </c>
+      <c r="D39" s="11">
+        <v>-153660.12</v>
+      </c>
+      <c r="E39" s="12">
+        <v>-1.3299999999999999E-2</v>
+      </c>
+      <c r="F39" s="11">
+        <v>20</v>
+      </c>
+      <c r="G39" s="11">
+        <v>11980700</v>
+      </c>
+      <c r="H39" s="11">
+        <v>11791977.970000001</v>
+      </c>
+      <c r="I39" s="11">
+        <v>-188722.03</v>
+      </c>
+      <c r="J39" s="12">
+        <v>-1.5800000000000002E-2</v>
+      </c>
+      <c r="K39" s="11">
+        <v>14</v>
+      </c>
+      <c r="L39" s="11">
+        <v>11935200</v>
+      </c>
+      <c r="M39" s="11">
+        <v>11934454.77</v>
+      </c>
+      <c r="N39" s="11">
+        <v>-745.23</v>
+      </c>
+      <c r="O39" s="12">
+        <v>-1E-4</v>
+      </c>
+      <c r="P39" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A40" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="11">
+        <v>188593300</v>
+      </c>
+      <c r="C40" s="11">
+        <v>188551675.69999999</v>
+      </c>
+      <c r="D40" s="11">
+        <v>-41624.32</v>
+      </c>
+      <c r="E40" s="12">
+        <v>-2.0000000000000001E-4</v>
+      </c>
+      <c r="F40" s="11">
+        <v>8</v>
+      </c>
+      <c r="G40" s="11">
+        <v>199130300</v>
+      </c>
+      <c r="H40" s="11">
+        <v>196755033.30000001</v>
+      </c>
+      <c r="I40" s="11">
+        <v>-2375266.69</v>
+      </c>
+      <c r="J40" s="12">
+        <v>-1.1900000000000001E-2</v>
+      </c>
+      <c r="K40" s="11">
+        <v>13</v>
+      </c>
+      <c r="L40" s="11">
+        <v>199954600</v>
+      </c>
+      <c r="M40" s="11">
+        <v>199954563.69999999</v>
+      </c>
+      <c r="N40" s="11">
+        <v>-36.250001009999998</v>
+      </c>
+      <c r="O40" s="12">
+        <v>0</v>
+      </c>
+      <c r="P40" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A41" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" s="11">
+        <v>512000</v>
+      </c>
+      <c r="C41" s="11">
+        <v>505017.37</v>
+      </c>
+      <c r="D41" s="11">
+        <v>-6982.63</v>
+      </c>
+      <c r="E41" s="12">
+        <v>-1.3599999999999999E-2</v>
+      </c>
+      <c r="F41" s="11">
+        <v>22</v>
+      </c>
+      <c r="G41" s="11">
+        <v>530500</v>
+      </c>
+      <c r="H41" s="11">
+        <v>524402.98</v>
+      </c>
+      <c r="I41" s="11">
+        <v>-6097.02</v>
+      </c>
+      <c r="J41" s="12">
+        <v>-1.15E-2</v>
+      </c>
+      <c r="K41" s="11">
+        <v>12</v>
+      </c>
+      <c r="L41" s="11">
+        <v>526200</v>
+      </c>
+      <c r="M41" s="11">
+        <v>504989.88</v>
+      </c>
+      <c r="N41" s="11">
+        <v>-21210.12</v>
+      </c>
+      <c r="O41" s="12">
+        <v>-4.0300000000000002E-2</v>
+      </c>
+      <c r="P41" s="11">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A42" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="11">
+        <v>30083200</v>
+      </c>
+      <c r="C42" s="11">
+        <v>29789104.379999999</v>
+      </c>
+      <c r="D42" s="11">
+        <v>-294095.62</v>
+      </c>
+      <c r="E42" s="12">
+        <v>-9.7999999999999997E-3</v>
+      </c>
+      <c r="F42" s="11">
+        <v>13</v>
+      </c>
+      <c r="G42" s="11">
+        <v>31040700</v>
+      </c>
+      <c r="H42" s="11">
+        <v>30793711.48</v>
+      </c>
+      <c r="I42" s="11">
+        <v>-246988.52</v>
+      </c>
+      <c r="J42" s="12">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+      <c r="K42" s="11">
+        <v>11</v>
+      </c>
+      <c r="L42" s="11">
+        <v>31282200</v>
+      </c>
+      <c r="M42" s="11">
+        <v>31282141.25</v>
+      </c>
+      <c r="N42" s="11">
+        <v>-58.75</v>
+      </c>
+      <c r="O42" s="12">
+        <v>0</v>
+      </c>
+      <c r="P42" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A43" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="11">
+        <v>12132200</v>
+      </c>
+      <c r="C43" s="11">
+        <v>12030494.1</v>
+      </c>
+      <c r="D43" s="11">
+        <v>-101705.9</v>
+      </c>
+      <c r="E43" s="12">
+        <v>-8.3999999999999995E-3</v>
+      </c>
+      <c r="F43" s="11">
+        <v>12</v>
+      </c>
+      <c r="G43" s="11">
+        <v>12735900</v>
+      </c>
+      <c r="H43" s="11">
+        <v>12685514.279999999</v>
+      </c>
+      <c r="I43" s="11">
+        <v>-50385.72</v>
+      </c>
+      <c r="J43" s="12">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="K43" s="11">
+        <v>10</v>
+      </c>
+      <c r="L43" s="11">
+        <v>12861300</v>
+      </c>
+      <c r="M43" s="11">
+        <v>12826009.609999999</v>
+      </c>
+      <c r="N43" s="11">
+        <v>-35290.39</v>
+      </c>
+      <c r="O43" s="12">
+        <v>-2.7000000000000001E-3</v>
+      </c>
+      <c r="P43" s="11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A44" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="11">
+        <v>927703100</v>
+      </c>
+      <c r="C44" s="11">
+        <v>920284264.70000005</v>
+      </c>
+      <c r="D44" s="11">
+        <v>-7418835.2699999996</v>
+      </c>
+      <c r="E44" s="12">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+      <c r="F44" s="11">
+        <v>11</v>
+      </c>
+      <c r="G44" s="11">
+        <v>979671000</v>
+      </c>
+      <c r="H44" s="11">
+        <v>977068513.5</v>
+      </c>
+      <c r="I44" s="11">
+        <v>-2602486.52</v>
+      </c>
+      <c r="J44" s="12">
+        <v>-2.7000000000000001E-3</v>
+      </c>
+      <c r="K44" s="11">
+        <v>9</v>
+      </c>
+      <c r="L44" s="11">
+        <v>989572900</v>
+      </c>
+      <c r="M44" s="11">
+        <v>984116289.39999998</v>
+      </c>
+      <c r="N44" s="11">
+        <v>-5456610.5899999999</v>
+      </c>
+      <c r="O44" s="12">
+        <v>-5.4999999999999997E-3</v>
+      </c>
+      <c r="P44" s="11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A45" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" s="11">
+        <v>409300</v>
+      </c>
+      <c r="C45" s="11">
+        <v>385908.52</v>
+      </c>
+      <c r="D45" s="11">
+        <v>-23391.48</v>
+      </c>
+      <c r="E45" s="12">
+        <v>-5.7099999999999998E-2</v>
+      </c>
+      <c r="F45" s="11">
+        <v>41</v>
+      </c>
+      <c r="G45" s="11">
+        <v>428500</v>
+      </c>
+      <c r="H45" s="11">
+        <v>427758.64</v>
+      </c>
+      <c r="I45" s="11">
+        <v>-741.36</v>
+      </c>
+      <c r="J45" s="12">
+        <v>-1.6999999999999999E-3</v>
+      </c>
+      <c r="K45" s="11">
+        <v>8</v>
+      </c>
+      <c r="L45" s="11">
+        <v>445200</v>
+      </c>
+      <c r="M45" s="11">
+        <v>445114.29</v>
+      </c>
+      <c r="N45" s="11">
+        <v>-85.71</v>
+      </c>
+      <c r="O45" s="12">
+        <v>-2.0000000000000001E-4</v>
+      </c>
+      <c r="P45" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A46" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46" s="11">
+        <v>70390700</v>
+      </c>
+      <c r="C46" s="11">
+        <v>70378426.719999999</v>
+      </c>
+      <c r="D46" s="11">
+        <v>-12273.28</v>
+      </c>
+      <c r="E46" s="12">
+        <v>-2.0000000000000001E-4</v>
+      </c>
+      <c r="F46" s="11">
+        <v>7</v>
+      </c>
+      <c r="G46" s="11">
+        <v>73467000</v>
+      </c>
+      <c r="H46" s="11">
+        <v>73442541.659999996</v>
+      </c>
+      <c r="I46" s="11">
+        <v>-24458.34</v>
+      </c>
+      <c r="J46" s="12">
+        <v>-2.9999999999999997E-4</v>
+      </c>
+      <c r="K46" s="11">
+        <v>7</v>
+      </c>
+      <c r="L46" s="11">
+        <v>75072800</v>
+      </c>
+      <c r="M46" s="11">
+        <v>75050829.180000007</v>
+      </c>
+      <c r="N46" s="11">
+        <v>-21970.82</v>
+      </c>
+      <c r="O46" s="12">
+        <v>-2.9999999999999997E-4</v>
+      </c>
+      <c r="P46" s="11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A47" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B47" s="11">
+        <v>6600700</v>
+      </c>
+      <c r="C47" s="11">
+        <v>6522480.46</v>
+      </c>
+      <c r="D47" s="11">
+        <v>-78219.539999999994</v>
+      </c>
+      <c r="E47" s="12">
+        <v>-1.1900000000000001E-2</v>
+      </c>
+      <c r="F47" s="11">
+        <v>15</v>
+      </c>
+      <c r="G47" s="11">
+        <v>7352500</v>
+      </c>
+      <c r="H47" s="11">
+        <v>7350464.0800000001</v>
+      </c>
+      <c r="I47" s="11">
+        <v>-2035.92</v>
+      </c>
+      <c r="J47" s="12">
+        <v>-2.9999999999999997E-4</v>
+      </c>
+      <c r="K47" s="11">
+        <v>6</v>
+      </c>
+      <c r="L47" s="11">
+        <v>7397200</v>
+      </c>
+      <c r="M47" s="11">
+        <v>7397093</v>
+      </c>
+      <c r="N47" s="11">
+        <v>-107</v>
+      </c>
+      <c r="O47" s="12">
+        <v>0</v>
+      </c>
+      <c r="P47" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A48" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48" s="11">
+        <v>124385900</v>
+      </c>
+      <c r="C48" s="11">
+        <v>124384360.2</v>
+      </c>
+      <c r="D48" s="11">
+        <v>-1539.840001</v>
+      </c>
+      <c r="E48" s="12">
+        <v>0</v>
+      </c>
+      <c r="F48" s="11">
+        <v>6</v>
+      </c>
+      <c r="G48" s="11">
+        <v>131849400</v>
+      </c>
+      <c r="H48" s="11">
+        <v>131839624.40000001</v>
+      </c>
+      <c r="I48" s="11">
+        <v>-9775.6299999999992</v>
+      </c>
+      <c r="J48" s="12">
+        <v>-1E-4</v>
+      </c>
+      <c r="K48" s="11">
+        <v>5</v>
+      </c>
+      <c r="L48" s="11">
+        <v>130621400</v>
+      </c>
+      <c r="M48" s="11">
+        <v>130621283.5</v>
+      </c>
+      <c r="N48" s="11">
+        <v>-116.46000100000001</v>
+      </c>
+      <c r="O48" s="12">
+        <v>0</v>
+      </c>
+      <c r="P48" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A49" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="11">
+        <v>0</v>
+      </c>
+      <c r="C49" s="11">
+        <v>0</v>
+      </c>
+      <c r="D49" s="11">
+        <v>0</v>
+      </c>
+      <c r="E49" s="12">
+        <v>0</v>
+      </c>
+      <c r="F49" s="11">
+        <v>2</v>
+      </c>
+      <c r="G49" s="11">
+        <v>0</v>
+      </c>
+      <c r="H49" s="11">
+        <v>0</v>
+      </c>
+      <c r="I49" s="11">
+        <v>0</v>
+      </c>
+      <c r="J49" s="12">
+        <v>0</v>
+      </c>
+      <c r="K49" s="11">
+        <v>1</v>
+      </c>
+      <c r="L49" s="11">
+        <v>375000</v>
+      </c>
+      <c r="M49" s="11">
+        <v>63771.91</v>
+      </c>
+      <c r="N49" s="11">
+        <v>-311228.09000000003</v>
+      </c>
+      <c r="O49" s="12">
+        <v>-0.82989999999999997</v>
+      </c>
+      <c r="P49" s="11">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A50" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" s="11">
+        <v>0</v>
+      </c>
+      <c r="C50" s="11">
+        <v>0</v>
+      </c>
+      <c r="D50" s="11">
+        <v>0</v>
+      </c>
+      <c r="E50" s="12">
+        <v>0</v>
+      </c>
+      <c r="F50" s="11">
+        <v>2</v>
+      </c>
+      <c r="G50" s="11">
+        <v>0</v>
+      </c>
+      <c r="H50" s="11">
+        <v>0</v>
+      </c>
+      <c r="I50" s="11">
+        <v>0</v>
+      </c>
+      <c r="J50" s="12">
+        <v>0</v>
+      </c>
+      <c r="K50" s="11">
+        <v>1</v>
+      </c>
+      <c r="L50" s="11">
+        <v>0</v>
+      </c>
+      <c r="M50" s="11">
+        <v>0</v>
+      </c>
+      <c r="N50" s="11">
+        <v>0</v>
+      </c>
+      <c r="O50" s="12">
+        <v>0</v>
+      </c>
+      <c r="P50" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A51" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" s="11">
+        <v>0</v>
+      </c>
+      <c r="C51" s="11">
+        <v>0</v>
+      </c>
+      <c r="D51" s="11">
+        <v>0</v>
+      </c>
+      <c r="E51" s="12">
+        <v>0</v>
+      </c>
+      <c r="F51" s="11">
+        <v>2</v>
+      </c>
+      <c r="G51" s="11">
+        <v>0</v>
+      </c>
+      <c r="H51" s="11">
+        <v>0</v>
+      </c>
+      <c r="I51" s="11">
+        <v>0</v>
+      </c>
+      <c r="J51" s="12">
+        <v>0</v>
+      </c>
+      <c r="K51" s="11">
+        <v>1</v>
+      </c>
+      <c r="L51" s="11">
+        <v>0</v>
+      </c>
+      <c r="M51" s="11">
+        <v>0</v>
+      </c>
+      <c r="N51" s="11">
+        <v>0</v>
+      </c>
+      <c r="O51" s="12">
+        <v>0</v>
+      </c>
+      <c r="P51" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A52" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52" s="11">
+        <v>832600</v>
+      </c>
+      <c r="C52" s="11">
+        <v>832600</v>
+      </c>
+      <c r="D52" s="11">
+        <v>0</v>
+      </c>
+      <c r="E52" s="12">
+        <v>0</v>
+      </c>
+      <c r="F52" s="11">
+        <v>2</v>
+      </c>
+      <c r="G52" s="11">
+        <v>859100</v>
+      </c>
+      <c r="H52" s="11">
+        <v>859100</v>
+      </c>
+      <c r="I52" s="11">
+        <v>0</v>
+      </c>
+      <c r="J52" s="12">
+        <v>0</v>
+      </c>
+      <c r="K52" s="11">
+        <v>1</v>
+      </c>
+      <c r="L52" s="11">
+        <v>843200</v>
+      </c>
+      <c r="M52" s="11">
+        <v>843200</v>
+      </c>
+      <c r="N52" s="11">
+        <v>0</v>
+      </c>
+      <c r="O52" s="12">
+        <v>0</v>
+      </c>
+      <c r="P52" s="11">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB99AC6-F6B8-4A26-96BE-D02EE21B4B6C}">
   <dimension ref="A1:B10"/>
   <sheetViews>

</xml_diff>